<commit_message>
Updated part numbers for 7x7 maze IR module cables.
</commit_message>
<xml_diff>
--- a/GridMaze/3_x_3_maze/3_x_3_maze_BOM.xlsx
+++ b/GridMaze/3_x_3_maze/3_x_3_maze_BOM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293911D5-7E7F-4B86-AF57-6C645913BD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D2CA57-4E33-4493-B4D9-54656F0871CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5490" yWindow="1110" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>